<commit_message>
Miglioramenti e pulizia generale
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/grid_template.xlsx
+++ b/src/main/resources/excel/grid_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A597BE1D-3F35-416F-86EF-DDEE39049A48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432540F2-1407-4FB6-B478-D14431D7D2AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{0D89AE90-92E1-409F-BB3E-50049C1CF02A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="master" var="items" lastCell="A3" direction="RIGHT")
+jx:each(items="items" var="String" lastCell="A3" direction="DOWN")</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -59,7 +84,7 @@
     <t>Strings Demo</t>
   </si>
   <si>
-    <t>${i}</t>
+    <t>${String}</t>
   </si>
 </sst>
 </file>
@@ -393,7 +418,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>